<commit_message>
meteogram patch and human friendly date stamp
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_3_dom.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_3_dom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B081D0-B9E4-1A4D-B94A-842C1F1E579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF25759-7186-6541-ACD2-AAD72B764B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2260" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="980" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,10 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,13 +191,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -235,19 +225,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -548,19 +535,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="L1" sqref="G1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -597,7 +583,7 @@
         <v>-102.8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -617,7 +603,7 @@
         <v>-103.593</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>24</v>
       </c>
@@ -636,12 +622,8 @@
       <c r="F4">
         <v>-104.158</v>
       </c>
-      <c r="L4" s="2">
-        <f>500000/3-50000</f>
-        <v>116666.66666666666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>30</v>
       </c>
@@ -661,7 +643,7 @@
         <v>-98.834999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -681,7 +663,7 @@
         <v>-103.54600000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -701,7 +683,7 @@
         <v>-105.383</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -721,7 +703,7 @@
         <v>-103.098</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -741,7 +723,7 @@
         <v>-102.01900000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -761,7 +743,7 @@
         <v>-105.38</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -781,7 +763,7 @@
         <v>-105.542</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -801,7 +783,7 @@
         <v>-102.175</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>14</v>
       </c>
@@ -821,7 +803,7 @@
         <v>-102.65</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -841,7 +823,7 @@
         <v>-102.518</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>18</v>
       </c>
@@ -861,7 +843,7 @@
         <v>-101.601</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>19</v>
       </c>

</xml_diff>